<commit_message>
27/04/25 2 - Lots of progress. Urls added to tiles. full darkmode capability
</commit_message>
<xml_diff>
--- a/test_sheets/audio/al12-shortcuts-macosx.xlsx
+++ b/test_sheets/audio/al12-shortcuts-macosx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WebProjects\cheatsheet\test_sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WebProjects\cheatsheet\test_sheets\audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1AB91F-2B8A-46B7-BC04-6B4ECE64A942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EFD2EE-C162-4520-B84E-282F4BEA2E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25920" yWindow="0" windowWidth="25635" windowHeight="17640" xr2:uid="{75DD2C60-600A-4108-92BA-0F29B3D1B6A1}"/>
+    <workbookView xWindow="14865" yWindow="4020" windowWidth="21600" windowHeight="11295" xr2:uid="{75DD2C60-600A-4108-92BA-0F29B3D1B6A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="161">
   <si>
     <t>Section</t>
   </si>
@@ -513,16 +513,30 @@
   </si>
   <si>
     <t>Focus on selected scene/track.</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=bhWJF9FlBqM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -545,16 +559,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -887,15 +906,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1EC5822-D226-416B-B4EC-FDC6D50B2C80}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -908,8 +927,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -922,8 +944,11 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -936,8 +961,9 @@
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -950,8 +976,9 @@
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -964,8 +991,9 @@
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -978,8 +1006,9 @@
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -992,8 +1021,11 @@
       <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1006,8 +1038,11 @@
       <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1020,8 +1055,11 @@
       <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1034,8 +1072,11 @@
       <c r="D10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1048,8 +1089,11 @@
       <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1062,8 +1106,11 @@
       <c r="D12" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1076,8 +1123,11 @@
       <c r="D13" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1090,8 +1140,11 @@
       <c r="D14" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -1104,8 +1157,11 @@
       <c r="D15" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E15" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1118,8 +1174,11 @@
       <c r="D16" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -1132,8 +1191,11 @@
       <c r="D17" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1146,8 +1208,11 @@
       <c r="D18" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -1160,8 +1225,11 @@
       <c r="D19" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
@@ -1174,8 +1242,11 @@
       <c r="D20" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E20" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -1188,8 +1259,11 @@
       <c r="D21" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -1202,8 +1276,11 @@
       <c r="D22" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
@@ -1216,8 +1293,11 @@
       <c r="D23" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E23" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -1230,8 +1310,11 @@
       <c r="D24" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E24" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
@@ -1244,8 +1327,11 @@
       <c r="D25" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>52</v>
       </c>
@@ -1258,8 +1344,11 @@
       <c r="D26" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E26" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
@@ -1272,8 +1361,11 @@
       <c r="D27" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E27" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>52</v>
       </c>
@@ -1286,8 +1378,11 @@
       <c r="D28" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E28" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>66</v>
       </c>
@@ -1300,8 +1395,11 @@
       <c r="D29" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E29" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>66</v>
       </c>
@@ -1314,8 +1412,11 @@
       <c r="D30" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E30" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>66</v>
       </c>
@@ -1328,8 +1429,11 @@
       <c r="D31" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E31" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>66</v>
       </c>
@@ -1342,8 +1446,11 @@
       <c r="D32" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E32" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>76</v>
       </c>
@@ -1356,8 +1463,11 @@
       <c r="D33" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E33" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
@@ -1370,8 +1480,11 @@
       <c r="D34" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E34" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
@@ -1384,8 +1497,11 @@
       <c r="D35" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E35" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>76</v>
       </c>
@@ -1398,8 +1514,11 @@
       <c r="D36" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E36" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>85</v>
       </c>
@@ -1412,8 +1531,11 @@
       <c r="D37" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E37" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>85</v>
       </c>
@@ -1426,8 +1548,11 @@
       <c r="D38" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E38" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
@@ -1440,8 +1565,11 @@
       <c r="D39" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E39" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>85</v>
       </c>
@@ -1454,8 +1582,11 @@
       <c r="D40" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E40" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -1468,8 +1599,11 @@
       <c r="D41" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E41" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>95</v>
       </c>
@@ -1482,8 +1616,11 @@
       <c r="D42" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E42" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>95</v>
       </c>
@@ -1496,8 +1633,11 @@
       <c r="D43" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E43" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>95</v>
       </c>
@@ -1510,8 +1650,11 @@
       <c r="D44" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E44" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>95</v>
       </c>
@@ -1524,8 +1667,11 @@
       <c r="D45" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E45" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>4</v>
       </c>
@@ -1538,8 +1684,11 @@
       <c r="D46" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E46" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>4</v>
       </c>
@@ -1552,8 +1701,11 @@
       <c r="D47" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E47" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>4</v>
       </c>
@@ -1566,8 +1718,11 @@
       <c r="D48" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E48" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>4</v>
       </c>
@@ -1580,8 +1735,11 @@
       <c r="D49" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E49" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>4</v>
       </c>
@@ -1594,8 +1752,11 @@
       <c r="D50" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E50" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>16</v>
       </c>
@@ -1608,8 +1769,11 @@
       <c r="D51" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E51" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>16</v>
       </c>
@@ -1622,8 +1786,11 @@
       <c r="D52" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E52" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>16</v>
       </c>
@@ -1636,8 +1803,11 @@
       <c r="D53" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E53" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>16</v>
       </c>
@@ -1650,8 +1820,11 @@
       <c r="D54" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E54" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>16</v>
       </c>
@@ -1664,8 +1837,11 @@
       <c r="D55" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E55" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>16</v>
       </c>
@@ -1678,8 +1854,11 @@
       <c r="D56" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E56" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>34</v>
       </c>
@@ -1692,8 +1871,11 @@
       <c r="D57" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E57" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>34</v>
       </c>
@@ -1706,8 +1888,11 @@
       <c r="D58" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E58" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>34</v>
       </c>
@@ -1720,8 +1905,11 @@
       <c r="D59" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E59" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>34</v>
       </c>
@@ -1734,8 +1922,11 @@
       <c r="D60" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E60" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>34</v>
       </c>
@@ -1748,8 +1939,11 @@
       <c r="D61" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E61" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>52</v>
       </c>
@@ -1762,8 +1956,11 @@
       <c r="D62" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E62" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>52</v>
       </c>
@@ -1776,8 +1973,11 @@
       <c r="D63" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E63" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>52</v>
       </c>
@@ -1790,8 +1990,11 @@
       <c r="D64" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E64" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>52</v>
       </c>
@@ -1804,8 +2007,11 @@
       <c r="D65" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E65" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>52</v>
       </c>
@@ -1818,8 +2024,11 @@
       <c r="D66" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E66" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
@@ -1832,8 +2041,11 @@
       <c r="D67" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E67" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
@@ -1846,8 +2058,11 @@
       <c r="D68" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E68" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>66</v>
       </c>
@@ -1860,8 +2075,11 @@
       <c r="D69" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E69" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>66</v>
       </c>
@@ -1874,8 +2092,11 @@
       <c r="D70" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E70" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>76</v>
       </c>
@@ -1888,8 +2109,11 @@
       <c r="D71" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E71" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>76</v>
       </c>
@@ -1902,8 +2126,11 @@
       <c r="D72" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E72" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>76</v>
       </c>
@@ -1916,8 +2143,11 @@
       <c r="D73" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E73" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>76</v>
       </c>
@@ -1930,8 +2160,11 @@
       <c r="D74" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E74" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>85</v>
       </c>
@@ -1944,8 +2177,11 @@
       <c r="D75" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E75" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>85</v>
       </c>
@@ -1958,8 +2194,11 @@
       <c r="D76" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E76" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>85</v>
       </c>
@@ -1972,8 +2211,11 @@
       <c r="D77" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E77" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>85</v>
       </c>
@@ -1986,8 +2228,11 @@
       <c r="D78" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E78" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>85</v>
       </c>
@@ -2000,8 +2245,11 @@
       <c r="D79" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E79" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>95</v>
       </c>
@@ -2014,8 +2262,11 @@
       <c r="D80" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E80" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>95</v>
       </c>
@@ -2028,8 +2279,9 @@
       <c r="D81" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E81" s="2"/>
+    </row>
+    <row r="82" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>95</v>
       </c>
@@ -2042,8 +2294,9 @@
       <c r="D82" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E82" s="2"/>
+    </row>
+    <row r="83" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>95</v>
       </c>
@@ -2056,8 +2309,9 @@
       <c r="D83" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>95</v>
       </c>
@@ -2070,8 +2324,14 @@
       <c r="D84" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="E84" s="2" t="s">
+        <v>160</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{F1582E82-9674-44FA-9702-F3116EAEE654}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>